<commit_message>
Versión de A_Z while
Se hizo una vesión para que buscara por letra en los filtros pero no funciona por
</commit_message>
<xml_diff>
--- a/Export/SAPnames.xlsx
+++ b/Export/SAPnames.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtotolhua\Documents\UiPath\SAPAutomation\Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F206C7D6-381E-41EA-8A02-F727CFC30B3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EF3DA3-1E5A-4F50-8692-F23B8D73535B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -339,9 +339,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="28.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>